<commit_message>
Changed cell lookup from ordinal position to absolute cell reference
</commit_message>
<xml_diff>
--- a/DataImporterTester/import.xlsx
+++ b/DataImporterTester/import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlowradSource\Custom Development\DataImporterServiceBroker\DataImporterTester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\DataImporterServiceBroker\DataImporterTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB35686-7978-4A67-9D9D-4241C41921EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ED11D7-19EE-4E4D-9E90-545946F7CA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3460" windowWidth="38400" windowHeight="8090" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22785" yWindow="5145" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -416,11 +416,12 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
@@ -470,9 +471,6 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
         <v>1.1000000000000001</v>
       </c>

</xml_diff>

<commit_message>
Decimal SmartObject properties will try to remove scientific notation before importing
</commit_message>
<xml_diff>
--- a/DataImporterTester/import.xlsx
+++ b/DataImporterTester/import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\DataImporterServiceBroker\DataImporterTester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Brokers\DataImporterServiceBroker\DataImporterTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ED11D7-19EE-4E4D-9E90-545946F7CA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42668F2-862F-4251-948C-2992504C98F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22785" yWindow="5145" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="5490" windowWidth="25920" windowHeight="15650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -416,32 +416,32 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -467,7 +467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -490,7 +490,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -498,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>2.2000000000000002</v>
+        <v>9.1328699200000002E-2</v>
       </c>
       <c r="E5" s="1">
         <v>37289</v>

</xml_diff>